<commit_message>
Mise à jour du gant interraction
mise à jour du gant
</commit_message>
<xml_diff>
--- a/Documentation/Gantt sans schéma.xlsx
+++ b/Documentation/Gantt sans schéma.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24240" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>A faire</t>
   </si>
@@ -159,8 +159,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +179,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,69 +287,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -355,7 +385,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,7 +459,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -464,7 +493,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,14 +668,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -659,519 +687,496 @@
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="19"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="21" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="11"/>
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="15" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="13" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="13" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="3"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F13" s="3"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="F11" s="2"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="F12" s="2"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="F13" s="2"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="22" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12" t="s">
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="12" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="11"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="11"/>
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12" t="s">
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="11"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="17"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="F21" s="2"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="F22" s="3"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="22" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="C25" s="13" t="s">
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="5"/>
+      <c r="C25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="8"/>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="C26" s="13" t="s">
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="5"/>
+      <c r="C26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13" t="s">
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="5"/>
+      <c r="B27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="5"/>
+      <c r="B28" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="22" t="s">
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="8"/>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="C29" s="13" t="s">
+      <c r="H28" s="30"/>
+      <c r="I28" s="31"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="5"/>
+      <c r="C29" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
-      <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="C30" s="13" t="s">
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="5"/>
+      <c r="C30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="8"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="5"/>
+      <c r="B31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="8"/>
-      <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="C32" s="13" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="12"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="5"/>
+      <c r="C32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="8"/>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="C33" s="13" t="s">
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="5"/>
+      <c r="C33" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="12"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="C34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="8"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F34" s="2"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="8"/>
-      <c r="O35" s="3"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="12"/>
+      <c r="O35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="C32:F32"/>
@@ -1188,14 +1193,41 @@
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1203,24 +1235,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à jour 01/12
</commit_message>
<xml_diff>
--- a/Documentation/Gantt sans schéma.xlsx
+++ b/Documentation/Gantt sans schéma.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>A faire</t>
   </si>
@@ -169,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +179,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -308,13 +302,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,12 +337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,14 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,15 +353,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -671,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -688,167 +673,167 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="17" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="18"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="19" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="11"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="13"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="11"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="13"/>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="13"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="22" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="13"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="22" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="13"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="22" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="13"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
       <c r="F11" s="2"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15">
       <c r="F12" s="2"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="13"/>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15">
       <c r="F13" s="2"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="13"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15">
@@ -858,9 +843,9 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -869,7 +854,7 @@
       <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -881,19 +866,19 @@
       <c r="D15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="13"/>
+      <c r="G15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="13"/>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="11"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
@@ -905,37 +890,37 @@
         <v>16</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="13"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="11"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="13"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="11"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="13"/>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="11"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -951,13 +936,13 @@
       <c r="F19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="13"/>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="11"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>22</v>
@@ -967,23 +952,23 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="13"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15">
       <c r="F21" s="2"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="13"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15">
       <c r="F22" s="3"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="13"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15">
@@ -993,9 +978,9 @@
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -1007,84 +992,86 @@
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="10" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="13"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="5"/>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="13"/>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="5"/>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="27"/>
+      <c r="I26" s="28"/>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="5"/>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="13"/>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="5"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="29" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="5"/>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="23"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
       <c r="G29" s="26" t="s">
         <v>42</v>
       </c>
@@ -1094,57 +1081,59 @@
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="5"/>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="29" t="s">
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="31"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="5"/>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="13"/>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="5"/>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="5"/>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="13"/>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15">
@@ -1152,9 +1141,9 @@
         <v>38</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="13"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="1:15">
@@ -1162,49 +1151,20 @@
         <v>40</v>
       </c>
       <c r="F35" s="2"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="13"/>
       <c r="O35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="G10:I10"/>
@@ -1221,13 +1181,42 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>